<commit_message>
Revised the text as data tutorial and the problem set
</commit_message>
<xml_diff>
--- a/Group, Coding Assignment, Leading Discussion/Group, Coding Assignment, Leading Discussion.xlsx
+++ b/Group, Coding Assignment, Leading Discussion/Group, Coding Assignment, Leading Discussion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jared_Edgerton\Dropbox\teaching_material\PSU\soda_501\Group, Coding Assignment, Leading Discussion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFB3245-1BA4-4D9D-8A90-3030206DF0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B011365-5236-4A13-A9CB-825704EE0A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{EC1FA02E-612C-494A-963C-FE1C97348D14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EC1FA02E-612C-494A-963C-FE1C97348D14}"/>
   </bookViews>
   <sheets>
     <sheet name="Group" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>Members</t>
   </si>
   <si>
-    <t>Rehab and Songtao</t>
-  </si>
-  <si>
     <t>Kei and Lesley</t>
   </si>
   <si>
@@ -89,6 +86,9 @@
   </si>
   <si>
     <t>Kaiwan</t>
+  </si>
+  <si>
+    <t>Rehab, Songtao, Jiahui</t>
   </si>
 </sst>
 </file>
@@ -462,13 +462,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA3E93E-82E4-4A88-9248-09907879C205}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,36 +476,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -521,106 +521,106 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -634,110 +634,110 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70ED5127-DBB8-4B1E-8DA2-EFF09F108950}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Revision to experiments problem set
</commit_message>
<xml_diff>
--- a/Group, Coding Assignment, Leading Discussion/Group, Coding Assignment, Leading Discussion.xlsx
+++ b/Group, Coding Assignment, Leading Discussion/Group, Coding Assignment, Leading Discussion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jared_Edgerton\Dropbox\teaching_material\PSU\soda_501\Group, Coding Assignment, Leading Discussion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B011365-5236-4A13-A9CB-825704EE0A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DF6A56-D79C-487D-820B-41FF27C0A9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EC1FA02E-612C-494A-963C-FE1C97348D14}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{EC1FA02E-612C-494A-963C-FE1C97348D14}"/>
   </bookViews>
   <sheets>
     <sheet name="Group" sheetId="1" r:id="rId1"/>
@@ -462,13 +462,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA3E93E-82E4-4A88-9248-09907879C205}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,7 +476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -484,7 +484,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -492,7 +492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -500,7 +500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -521,9 +521,9 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -531,12 +531,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -544,12 +544,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -557,7 +557,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -565,7 +565,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -573,7 +573,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -581,12 +581,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -594,12 +594,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -607,7 +607,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -615,12 +615,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -634,13 +634,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70ED5127-DBB8-4B1E-8DA2-EFF09F108950}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -648,12 +648,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -661,7 +661,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -669,7 +669,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -677,15 +677,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -693,17 +690,20 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -711,17 +711,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -729,7 +729,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -737,7 +737,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>

</xml_diff>